<commit_message>
Added the logic to store the work item type in the config file
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\UiPath\ACMESystem1_ProcessVendorInvoice\ACMESystem1_ProcessVendorInvoice_Dispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\UiPath\ACMESystem1_ProcessVendorInvoice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E6780E-8B44-43CC-AC14-4810BFCAFFFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F15C2A5-5D82-4584-881D-9DC8014F7D5C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -187,6 +187,15 @@
   </si>
   <si>
     <t>ACMESystem1_ProcessVendorInvoice_Dispatcher</t>
+  </si>
+  <si>
+    <t>Type of the work items to be processed by the BOT (E.g: WI2, WI3 e.t.c)</t>
+  </si>
+  <si>
+    <t>Process_WorkItemsType</t>
+  </si>
+  <si>
+    <t>WI2</t>
   </si>
 </sst>
 </file>
@@ -1665,10 +1674,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z988"/>
+  <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1828,67 +1837,81 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="4">
-        <v>587</v>
+        <v>38</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="4">
+        <v>587</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2856,6 +2879,8 @@
     <row r="986" ht="14.25" customHeight="1"/>
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
+    <row r="989" ht="14.25" customHeight="1"/>
+    <row r="990" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
initial release for performer & few enhance,emnts for dispatcher
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\UiPath\ACMESystem1_ProcessVendorInvoice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F15C2A5-5D82-4584-881D-9DC8014F7D5C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C1B21E-BC26-4421-AC04-30F90698D1F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>System exception.</t>
-  </si>
-  <si>
-    <t>logF_BusinessProcessName</t>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -196,6 +193,15 @@
   </si>
   <si>
     <t>WI2</t>
+  </si>
+  <si>
+    <t>ACMESystem1_ProcessVendorInvoice_Performer</t>
+  </si>
+  <si>
+    <t>logF_DispatcherProcessName</t>
+  </si>
+  <si>
+    <t>logF_PerformerProcessName</t>
   </si>
 </sst>
 </file>
@@ -593,13 +599,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="88.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
@@ -641,38 +647,48 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="30">
       <c r="A4" s="5" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="30">
+      <c r="A5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1676,7 +1692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z990"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -1730,7 +1746,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -1762,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1784,7 +1800,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1795,7 +1811,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1806,7 +1822,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1816,24 +1832,24 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="C12" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
@@ -1843,13 +1859,13 @@
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>56</v>
-      </c>
       <c r="C15" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
@@ -1859,57 +1875,57 @@
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" s="4">
         <v>587</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2911,7 +2927,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
All the framework logic completed
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\UiPath\ACMESystem1_ProcessVendorInvoice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C1B21E-BC26-4421-AC04-30F90698D1F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60F8529-F726-4E02-A16B-1B45DE447C1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -192,9 +192,6 @@
     <t>Process_WorkItemsType</t>
   </si>
   <si>
-    <t>WI2</t>
-  </si>
-  <si>
     <t>ACMESystem1_ProcessVendorInvoice_Performer</t>
   </si>
   <si>
@@ -202,6 +199,9 @@
   </si>
   <si>
     <t>logF_PerformerProcessName</t>
+  </si>
+  <si>
+    <t>WI3</t>
   </si>
 </sst>
 </file>
@@ -599,7 +599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -669,7 +669,7 @@
     </row>
     <row r="4" spans="1:26" ht="30">
       <c r="A4" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>52</v>
@@ -680,10 +680,10 @@
     </row>
     <row r="5" spans="1:26" ht="30">
       <c r="A5" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>21</v>
@@ -1692,8 +1692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z990"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1743,7 +1743,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>23</v>
@@ -1862,7 +1862,7 @@
         <v>54</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
Republishing after code cleanup
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\UiPath\ACMESystem1_ProcessVendorInvoice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60F8529-F726-4E02-A16B-1B45DE447C1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33EBC672-B248-4239-A08C-A452EFD384F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -202,6 +202,24 @@
   </si>
   <si>
     <t>WI3</t>
+  </si>
+  <si>
+    <t>ACMESystem1_WorkItemURL</t>
+  </si>
+  <si>
+    <t>URL to open a specific work item in the ACME System 1 portal</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/work-items/{0}</t>
+  </si>
+  <si>
+    <t>Default path to store the downloaded files</t>
+  </si>
+  <si>
+    <t>D:\UiPath Project Space\ACMESystem1_ProcessVendorInvoice\Invoices</t>
+  </si>
+  <si>
+    <t>Process_DefaultDownloadLocation</t>
   </si>
 </sst>
 </file>
@@ -253,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -283,6 +301,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1690,10 +1709,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z990"/>
+  <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1853,83 +1872,103 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="2"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="2"/>
+      <c r="A14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="A15" s="2"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
+      <c r="A16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>38</v>
+        <v>64</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>63</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>42</v>
-      </c>
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="4">
-        <v>587</v>
+        <v>37</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="4">
+        <v>587</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2897,6 +2936,8 @@
     <row r="988" ht="14.25" customHeight="1"/>
     <row r="989" ht="14.25" customHeight="1"/>
     <row r="990" ht="14.25" customHeight="1"/>
+    <row r="991" ht="14.25" customHeight="1"/>
+    <row r="992" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>